<commit_message>
Updates to the UI and general refactoring (supporting WPF). Added wrapper functions for forecast analytics.
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/R Types Tests.xlsx
+++ b/ExcelRAddIn/Tests/R Types Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4058FA-409E-40EF-B110-9A01ED6561A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D96B91-A8A0-49D2-B6D6-5626EB00057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="852" firstSheet="2" activeTab="8" xr2:uid="{5877FA5A-76F9-4C4A-95F7-F8E57366BB43}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="852" firstSheet="10" activeTab="19" xr2:uid="{5877FA5A-76F9-4C4A-95F7-F8E57366BB43}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Types" sheetId="18" r:id="rId1"/>
@@ -1041,9 +1041,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1081,7 +1081,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1187,7 +1187,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1329,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1340,7 +1340,7 @@
   <dimension ref="B1:Q60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,43 +1397,43 @@
       </c>
       <c r="F2" cm="1">
         <f t="array" ref="F2">_xll.RScript.Evaluate($E$2&amp;"["&amp;F1&amp;"]")</f>
-        <v>-1.0579444978294112</v>
+        <v>-1.1880159611636512</v>
       </c>
       <c r="G2" cm="1">
         <f t="array" ref="G2">_xll.RScript.Evaluate($E$2&amp;"["&amp;G1&amp;"]")</f>
-        <v>-0.34675700843334811</v>
+        <v>-0.14831709096571422</v>
       </c>
       <c r="H2" cm="1">
         <f t="array" ref="H2">_xll.RScript.Evaluate($E$2&amp;"["&amp;H1&amp;"]")</f>
-        <v>-1.3914632267915907</v>
+        <v>0.39898072850752042</v>
       </c>
       <c r="I2" cm="1">
         <f t="array" ref="I2">_xll.RScript.Evaluate($E$2&amp;"["&amp;I1&amp;"]")</f>
-        <v>-0.51979432070762666</v>
+        <v>0.12325104199573529</v>
       </c>
       <c r="J2" cm="1">
         <f t="array" ref="J2">_xll.RScript.Evaluate($E$2&amp;"["&amp;J1&amp;"]")</f>
-        <v>-0.26026432623747425</v>
+        <v>0.66194300195975542</v>
       </c>
       <c r="K2" cm="1">
         <f t="array" ref="K2">_xll.RScript.Evaluate($E$2&amp;"["&amp;K1&amp;"]")</f>
-        <v>-1.8307278764434405</v>
+        <v>0.66681371838657433</v>
       </c>
       <c r="L2" cm="1">
         <f t="array" ref="L2">_xll.RScript.Evaluate($E$2&amp;"["&amp;L1&amp;"]")</f>
-        <v>1.038726491394004</v>
+        <v>-1.5209845574473024</v>
       </c>
       <c r="M2" cm="1">
         <f t="array" ref="M2">_xll.RScript.Evaluate($E$2&amp;"["&amp;M1&amp;"]")</f>
-        <v>0.24997500890044486</v>
+        <v>-0.19923384758078849</v>
       </c>
       <c r="N2" cm="1">
         <f t="array" ref="N2">_xll.RScript.Evaluate($E$2&amp;"["&amp;N1&amp;"]")</f>
-        <v>0.2799300143278371</v>
+        <v>0.20190649829949189</v>
       </c>
       <c r="O2" cm="1">
         <f t="array" ref="O2">_xll.RScript.Evaluate($E$2&amp;"["&amp;O1&amp;"]")</f>
-        <v>-0.49092292086657291</v>
+        <v>-0.44047867839884547</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
@@ -1553,43 +1553,43 @@
       </c>
       <c r="F5" t="str" cm="1">
         <f t="array" ref="F5">_xll.RScript.Evaluate($E$5&amp;"["&amp;F1&amp;"]")</f>
-        <v>-0.44253884643939-0.570844745935023i</v>
+        <v>-0.333705621073604+0.639802141545883i</v>
       </c>
       <c r="G5" t="str" cm="1">
         <f t="array" ref="G5">_xll.RScript.Evaluate($E$5&amp;"["&amp;G1&amp;"]")</f>
-        <v>1.81416921323255-1.15830725379693i</v>
+        <v>0.462919588283699-0.700618026485648i</v>
       </c>
       <c r="H5" t="str" cm="1">
         <f t="array" ref="H5">_xll.RScript.Evaluate($E$5&amp;"["&amp;H1&amp;"]")</f>
-        <v>0.281303416294633-0.446452058394078i</v>
+        <v>0.376810911043259+2.25697250809625i</v>
       </c>
       <c r="I5" t="str" cm="1">
         <f t="array" ref="I5">_xll.RScript.Evaluate($E$5&amp;"["&amp;I1&amp;"]")</f>
-        <v>-0.172986034907509-0.164156818046041i</v>
+        <v>0.534028526624503+1.22188980902137i</v>
       </c>
       <c r="J5" t="str" cm="1">
         <f t="array" ref="J5">_xll.RScript.Evaluate($E$5&amp;"["&amp;J1&amp;"]")</f>
-        <v>0.508322077700328-1.17624575213297i</v>
+        <v>2.36514333388565-0.401828513903769i</v>
       </c>
       <c r="K5" t="str" cm="1">
         <f t="array" ref="K5">_xll.RScript.Evaluate($E$5&amp;"["&amp;K1&amp;"]")</f>
-        <v>0.643853528270414-0.814292700875728i</v>
+        <v>-0.17272202036455+0.368944610077771i</v>
       </c>
       <c r="L5" t="str" cm="1">
         <f t="array" ref="L5">_xll.RScript.Evaluate($E$5&amp;"["&amp;L1&amp;"]")</f>
-        <v>0.574058130524811-1.70537384139491i</v>
+        <v>0.0241603518073429-0.866381113796704i</v>
       </c>
       <c r="M5" t="str" cm="1">
         <f t="array" ref="M5">_xll.RScript.Evaluate($E$5&amp;"["&amp;M1&amp;"]")</f>
-        <v>-1.02849697179285-0.632795168208102i</v>
+        <v>-0.0831477635497377-0.88714291903732i</v>
       </c>
       <c r="N5" t="str" cm="1">
         <f t="array" ref="N5">_xll.RScript.Evaluate($E$5&amp;"["&amp;N1&amp;"]")</f>
-        <v>0.79420057598073+0.479990556664285i</v>
+        <v>-0.193696321186678+0.314861612732435i</v>
       </c>
       <c r="O5" t="str" cm="1">
         <f t="array" ref="O5">_xll.RScript.Evaluate($E$5&amp;"["&amp;O1&amp;"]")</f>
-        <v>-0.477098313745436-0.710496534414749i</v>
+        <v>-2.19699868926359-1.79484425996288i</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
@@ -7870,7 +7870,7 @@
   <dimension ref="D2:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8109,8 +8109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5F1B9E-7F32-4C1B-AD03-048C852061EA}">
   <dimension ref="B2:T327"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8340,7 +8340,7 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" t="str" cm="1">
-        <f t="array" ref="B27">_xll.RScript.CreateDataFrame("sales", TableSalesData[], TableSalesData[#Headers], D25:J25)</f>
+        <f t="array" ref="B27">_xll.RScript.CreateDataFrame("sales", TableSalesData[], TableSalesData[#Headers])</f>
         <v>sales</v>
       </c>
       <c r="D27" t="s">
@@ -22599,10 +22599,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE3A425-1B3A-48E4-81F6-708C847B230F}">
-  <dimension ref="C2:N102"/>
+  <dimension ref="C1:N102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22611,9 +22611,12 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D1" s="1"/>
+    </row>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2">_xll.RScript.CreateVector("vcplx1", C3:C102, "Complex")</f>
+        <f t="array" ref="C2">_xll.RScript.CreateVector("vcplx1", C3:C102)</f>
         <v>vcplx1</v>
       </c>
       <c r="G2" t="s">
@@ -27515,7 +27518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD336D55-5F31-4FE9-B37C-75EEC4381E9A}">
   <dimension ref="B2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>